<commit_message>
changed student registration as per the database requirements
</commit_message>
<xml_diff>
--- a/ExcelData.xlsx
+++ b/ExcelData.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,20 +452,106 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>18r21a12a0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Md Zikrullah</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>zikrullah@omnia.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>18r21a1280</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Vivek Jandhyala</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>vivek@omnia.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>18r21a1290</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>kota Srikar</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>kotasrikar009@gmail.com</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>IT</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>18r21a1298</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MD Q Arshad</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>arshad@omnia.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>2022</t>
         </is>

</xml_diff>